<commit_message>
word repeating more frequently
</commit_message>
<xml_diff>
--- a/单词库.xlsx
+++ b/单词库.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>english</t>
   </si>
@@ -37,127 +37,184 @@
     <t>chinese</t>
   </si>
   <si>
-    <t>abandon</t>
-  </si>
-  <si>
-    <t>v 扔弃（地位等），离弃（家园）</t>
-  </si>
-  <si>
-    <t>abhor</t>
-  </si>
-  <si>
-    <t>v 憎恶，厌恶，嫌弃</t>
-  </si>
-  <si>
-    <t>abnormal</t>
-  </si>
-  <si>
-    <t>a 反常的，变态的，不规则的</t>
-  </si>
-  <si>
-    <t>abroad</t>
-  </si>
-  <si>
-    <t>1 ad 到国外，在海外
-2 n 国外，海外</t>
-  </si>
-  <si>
-    <t>abrupt</t>
-  </si>
-  <si>
-    <t>a 突然的，生硬的</t>
-  </si>
-  <si>
-    <t>absent</t>
-  </si>
-  <si>
-    <t>a 不在的，缺席的</t>
-  </si>
-  <si>
-    <t>absorb</t>
-  </si>
-  <si>
-    <t>v 吸收</t>
-  </si>
-  <si>
-    <t>abstract</t>
-  </si>
-  <si>
-    <t>a&amp;n 抽象（的）</t>
-  </si>
-  <si>
-    <t>absurd</t>
-  </si>
-  <si>
-    <t>a 不合理的；荒谬的</t>
-  </si>
-  <si>
-    <t>abundant</t>
-  </si>
-  <si>
-    <t>a 丰富的，大量的</t>
-  </si>
-  <si>
-    <t>abuse</t>
-  </si>
-  <si>
-    <t>n&amp;v 滥用，乱用</t>
-  </si>
-  <si>
-    <t>academy</t>
-  </si>
-  <si>
-    <t>n 学会，研究院</t>
-  </si>
-  <si>
-    <t>accelerate</t>
-  </si>
-  <si>
-    <t>v 加速；催促，促进</t>
-  </si>
-  <si>
-    <t>access</t>
-  </si>
-  <si>
-    <t>1 n 进路，入口
-2 v 接近</t>
-  </si>
-  <si>
-    <t>accident</t>
-  </si>
-  <si>
-    <t>n 故障，事故，偶发事件；偶然</t>
-  </si>
-  <si>
-    <t>acclaim</t>
-  </si>
-  <si>
-    <t>n 喝彩，欢呼</t>
-  </si>
-  <si>
-    <t>accommodate</t>
-  </si>
-  <si>
-    <t>1 v 适应，调节
-2 v 留宿，招待</t>
-  </si>
-  <si>
-    <t>accompany</t>
-  </si>
-  <si>
-    <t>v 陪伴；伴奏</t>
-  </si>
-  <si>
-    <t>accomplish</t>
-  </si>
-  <si>
-    <t>v 成就，完成；贯彻（计划等）；达到（目的）；实行</t>
-  </si>
-  <si>
-    <t>accord</t>
-  </si>
-  <si>
-    <t>v 一致，与……符合（with）</t>
+    <t>call</t>
+  </si>
+  <si>
+    <t>v./n.把…叫做,打电话,召集n.拜访</t>
+  </si>
+  <si>
+    <t>specification</t>
+  </si>
+  <si>
+    <t>n.详述, 规格</t>
+  </si>
+  <si>
+    <t>ingenuity</t>
+  </si>
+  <si>
+    <t>n.机灵, 独创性</t>
+  </si>
+  <si>
+    <t>unpleasant</t>
+  </si>
+  <si>
+    <t>a.不愉快的,不合意的</t>
+  </si>
+  <si>
+    <t>overtake</t>
+  </si>
+  <si>
+    <t>vt.追上,超过,突然降临于,意外地碰上</t>
+  </si>
+  <si>
+    <t>binge</t>
+  </si>
+  <si>
+    <t>n.狂闹, 狂欢</t>
+  </si>
+  <si>
+    <t>deviation</t>
+  </si>
+  <si>
+    <t>n.背离,偏离,误差</t>
+  </si>
+  <si>
+    <t>graceful</t>
+  </si>
+  <si>
+    <t>a.优美的</t>
+  </si>
+  <si>
+    <t>sailor</t>
+  </si>
+  <si>
+    <t>n.海员, 水手</t>
+  </si>
+  <si>
+    <t>dumb</t>
+  </si>
+  <si>
+    <t>a.哑的,沉默的</t>
+  </si>
+  <si>
+    <t>ether</t>
+  </si>
+  <si>
+    <t>n.天空醚, 大气</t>
+  </si>
+  <si>
+    <t>substantially</t>
+  </si>
+  <si>
+    <t>ad.大体上,本质上</t>
+  </si>
+  <si>
+    <t>railway</t>
+  </si>
+  <si>
+    <t>n.铁路</t>
+  </si>
+  <si>
+    <t>gravitational</t>
+  </si>
+  <si>
+    <t>a.重力的, 引力作用的</t>
+  </si>
+  <si>
+    <t>encase</t>
+  </si>
+  <si>
+    <t>vt.装入, 包住,围绕</t>
+  </si>
+  <si>
+    <t>beater</t>
+  </si>
+  <si>
+    <t>n.搅拌器,敲打者</t>
+  </si>
+  <si>
+    <t>explorer</t>
+  </si>
+  <si>
+    <t>n.探险者</t>
+  </si>
+  <si>
+    <t>rapport</t>
+  </si>
+  <si>
+    <t>n.和谐, 亲善</t>
+  </si>
+  <si>
+    <t>gunfire</t>
+  </si>
+  <si>
+    <t>n.炮火</t>
+  </si>
+  <si>
+    <t>bedpan</t>
+  </si>
+  <si>
+    <t>n.便盆, 睡床用脚炉</t>
+  </si>
+  <si>
+    <t>swell</t>
+  </si>
+  <si>
+    <t>v.(使)膨胀, 增大</t>
+  </si>
+  <si>
+    <t>profoundly</t>
+  </si>
+  <si>
+    <t>ad.深深地, 衷心地</t>
+  </si>
+  <si>
+    <t>excrete</t>
+  </si>
+  <si>
+    <t>vt.排泄, 分泌</t>
+  </si>
+  <si>
+    <t>uniquely</t>
+  </si>
+  <si>
+    <t>adv独特地, 唯一地</t>
+  </si>
+  <si>
+    <t>homo</t>
+  </si>
+  <si>
+    <t>n.人, 同性恋者</t>
+  </si>
+  <si>
+    <t>albedo</t>
+  </si>
+  <si>
+    <t>n.[天文](星体)反照率</t>
+  </si>
+  <si>
+    <t>cool</t>
+  </si>
+  <si>
+    <t>v.冷却,(使)冷静adj. 冷静的,凉爽的</t>
+  </si>
+  <si>
+    <t>magnitude</t>
+  </si>
+  <si>
+    <t>n.大小, 数量,量级</t>
+  </si>
+  <si>
+    <t>rearrange</t>
+  </si>
+  <si>
+    <t>vt.再排列,重新整理</t>
+  </si>
+  <si>
+    <t>president</t>
+  </si>
+  <si>
+    <t>n.总统,会长,(大学)校长,董事长</t>
   </si>
 </sst>
 </file>
@@ -170,13 +227,19 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
     </font>
     <font>
       <u/>
@@ -517,12 +580,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -643,133 +721,133 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -777,7 +855,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1091,10 +1169,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="1"/>
@@ -1107,164 +1185,244 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" t="s">
+    <row r="2" ht="80.65" spans="1:2">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" t="s">
+    <row r="3" ht="32.25" spans="1:2">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" t="s">
+    <row r="4" ht="32.25" spans="1:2">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" ht="67.5" spans="1:2">
-      <c r="A5" t="s">
+    <row r="5" ht="48.4" spans="1:2">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" t="s">
+    <row r="6" ht="80.65" spans="1:2">
+      <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" t="s">
+    <row r="7" ht="32.25" spans="1:2">
+      <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" t="s">
+    <row r="8" ht="48.4" spans="1:2">
+      <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" t="s">
+    <row r="9" ht="16.15" spans="1:2">
+      <c r="A9" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" t="s">
+    <row r="10" ht="32.25" spans="1:2">
+      <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" t="s">
+    <row r="11" ht="32.25" spans="1:2">
+      <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" t="s">
+    <row r="12" ht="32.25" spans="1:2">
+      <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" t="s">
+    <row r="13" ht="48.4" spans="1:2">
+      <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" t="s">
+    <row r="14" ht="16.15" spans="1:2">
+      <c r="A14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" ht="40.5" spans="1:2">
-      <c r="A15" t="s">
+    <row r="15" ht="48.4" spans="1:2">
+      <c r="A15" s="1" t="s">
         <v>28</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" t="s">
+    <row r="16" ht="48.4" spans="1:2">
+      <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" t="s">
+    <row r="17" ht="48.4" spans="1:2">
+      <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="18" ht="54" spans="1:2">
-      <c r="A18" t="s">
+    <row r="18" ht="32.25" spans="1:2">
+      <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" t="s">
+    <row r="19" ht="32.25" spans="1:2">
+      <c r="A19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" t="s">
+    <row r="20" ht="16.15" spans="1:2">
+      <c r="A20" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" t="s">
+    <row r="21" ht="48.4" spans="1:2">
+      <c r="A21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="1" t="s">
         <v>41</v>
+      </c>
+    </row>
+    <row r="22" ht="32.25" spans="1:2">
+      <c r="A22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="23" ht="48.4" spans="1:2">
+      <c r="A23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="24" ht="32.25" spans="1:2">
+      <c r="A24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" ht="48.4" spans="1:2">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="26" ht="32.25" spans="1:2">
+      <c r="A26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="27" ht="64.5" spans="1:2">
+      <c r="A27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" ht="80.65" spans="1:2">
+      <c r="A28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" ht="48.4" spans="1:2">
+      <c r="A29" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" ht="48.4" spans="1:2">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" ht="64.5" spans="1:2">
+      <c r="A31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>